<commit_message>
add on competence and modif on index page
</commit_message>
<xml_diff>
--- a/excel/Excel_BTS_Portfolio.xlsx
+++ b/excel/Excel_BTS_Portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugo\OneDrive\Bureau\PERSO\PORTFOLIO\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157314EE-B007-40CF-8571-F509F68783F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373BC9AF-F731-4469-B7B0-2977C7DE2422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -50,16 +50,10 @@
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
   </si>
   <si>
-    <t xml:space="preserve">N° candidat : </t>
-  </si>
-  <si>
     <t>Centre de formation : EPSI Lille</t>
   </si>
   <si>
     <t>Option :</t>
-  </si>
-  <si>
-    <t>▢ SISR</t>
   </si>
   <si>
     <t>Compétences mises en œuvre
@@ -130,60 +124,21 @@
 </t>
   </si>
   <si>
-    <t>Dec 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Création différents jeux Python </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Création Base de Données UML </t>
-  </si>
-  <si>
-    <t>Fev 23</t>
-  </si>
-  <si>
-    <t>Structure de Données</t>
-  </si>
-  <si>
     <t>Commande Base de données SQL</t>
   </si>
   <si>
     <t>Réalisations en milieu professionnel en cours de première année</t>
   </si>
   <si>
-    <t xml:space="preserve">Apprentissage Javascript </t>
-  </si>
-  <si>
-    <t>Réalisation de Drag and Drop Javascript</t>
-  </si>
-  <si>
-    <t>Réalisation QCM Javascript</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Réalisation Texte à trou Javascript avec selection ou ecriture réponse </t>
-  </si>
-  <si>
     <t>Realisation page Web de Commande en PHP</t>
   </si>
   <si>
     <t>X SLAM</t>
   </si>
   <si>
-    <t xml:space="preserve">TP UI/UX </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP Meteoapp </t>
-  </si>
-  <si>
-    <t>Réalisation du PortFolio</t>
-  </si>
-  <si>
     <t>NOM et prénom : Hochart Hugo</t>
   </si>
   <si>
-    <t>Adresse URL du portfolio : hochart.heb3.org</t>
-  </si>
-  <si>
     <t>Réalisation de gestionnaire de stock en HTML/CSS/PhpMyAdmin</t>
   </si>
   <si>
@@ -196,10 +151,6 @@
     <t>Gestion de tickets avec GLPI</t>
   </si>
   <si>
-    <t xml:space="preserve">Réalisation en cours de formation 2ème année
-</t>
-  </si>
-  <si>
     <t>STAGE EFFECTUE CHEZ GNOSYS EXPERIMENTAL</t>
   </si>
   <si>
@@ -209,30 +160,18 @@
     <t>Création d'une page Emailing</t>
   </si>
   <si>
-    <t>Page Crud Backend</t>
-  </si>
-  <si>
     <t>Serveur Web, FTP, DNS</t>
   </si>
   <si>
-    <t>Gestionnaire de commande python</t>
-  </si>
-  <si>
     <t>Gestion Agence de Voyage SQL</t>
   </si>
   <si>
     <t>Création UML Amazon</t>
   </si>
   <si>
-    <t>Réalisations en mil+A22:H46ieu professionnel en cours de première année</t>
-  </si>
-  <si>
     <t>Création d'un poullailler en Python</t>
   </si>
   <si>
-    <t>Création d'algorithme</t>
-  </si>
-  <si>
     <t>Projet de commande de Sandwich en python</t>
   </si>
   <si>
@@ -258,6 +197,84 @@
   </si>
   <si>
     <t xml:space="preserve">Création d'un site e-commerce de vente de chaussure en React </t>
+  </si>
+  <si>
+    <t>Application de stock</t>
+  </si>
+  <si>
+    <t>Projet Agenda</t>
+  </si>
+  <si>
+    <t>Réalisations en milieu professionnel en cours de deuxième année</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://hugo-hochart.web-edu.fr/</t>
+  </si>
+  <si>
+    <t>N° candidat :  02047327769</t>
+  </si>
+  <si>
+    <t>22/11/22 au 08/12/22</t>
+  </si>
+  <si>
+    <t>16/01/23 au 17/01/23</t>
+  </si>
+  <si>
+    <t>20/02/23 au 26/04/23</t>
+  </si>
+  <si>
+    <t>20/02/23 au 21/02/23</t>
+  </si>
+  <si>
+    <t>09/02/23 au 23/02/23</t>
+  </si>
+  <si>
+    <t>20/03/23 au 26/06/23</t>
+  </si>
+  <si>
+    <t>25/09/23 au 25/10/23</t>
+  </si>
+  <si>
+    <t>10/12/23 au 25/04/24</t>
+  </si>
+  <si>
+    <t>02/12/23 au 18/12/23</t>
+  </si>
+  <si>
+    <t>03/11/23 au 15/11/23</t>
+  </si>
+  <si>
+    <t>05/12/23 au 20/03/24</t>
+  </si>
+  <si>
+    <t>18/03/24 au 09/04/24</t>
+  </si>
+  <si>
+    <t>24/02/24 au 08/03/24</t>
+  </si>
+  <si>
+    <t>03/03/24 au 27/04/24</t>
+  </si>
+  <si>
+    <t>10/11/23 au 22/12/23</t>
+  </si>
+  <si>
+    <t>20/03/23 au 10/04/23</t>
+  </si>
+  <si>
+    <t>16/01/23 au 20/01/23</t>
+  </si>
+  <si>
+    <t>10/11/22 au 16/01/23</t>
+  </si>
+  <si>
+    <t>20/02/23 au 07/03/23</t>
+  </si>
+  <si>
+    <t>15/05/2023 au 23/06/2023</t>
+  </si>
+  <si>
+    <t>02/01/2024 au 23/02/2024</t>
   </si>
 </sst>
 </file>
@@ -335,19 +352,18 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,18 +378,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -388,30 +398,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -512,148 +498,12 @@
         <color theme="2" tint="-0.749992370372631"/>
       </diagonal>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -670,169 +520,145 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1143,140 +969,140 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ97"/>
+  <dimension ref="A1:AQ77"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" style="1" customWidth="1"/>
     <col min="3" max="8" width="18.6640625" style="1" customWidth="1"/>
-    <col min="9" max="43" width="10.88671875" customWidth="1"/>
+    <col min="9" max="12" width="10.88671875" customWidth="1"/>
+    <col min="13" max="13" width="20.77734375" customWidth="1"/>
+    <col min="14" max="43" width="10.88671875" customWidth="1"/>
     <col min="44" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="2" spans="1:43" ht="40.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="H1" s="38"/>
+    </row>
+    <row r="2" spans="1:43" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="46"/>
     </row>
     <row r="3" spans="1:43" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
+      <c r="A3" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="41"/>
+      <c r="H3" s="42"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12" t="s">
+      <c r="G4" s="11"/>
+      <c r="H4" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="42"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="B6" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="30"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="C6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="E6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="F6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="G6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="H6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="15" t="s">
+    </row>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="325.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="43"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="32" t="s">
+      <c r="D7" s="13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="325.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="16" t="s">
+      <c r="E7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="F7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="G7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="H7" s="19" t="s">
         <v>18</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="33" t="s">
-        <v>20</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1315,16 +1141,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="35"/>
+      <c r="A8" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="36"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1362,14 +1188,14 @@
       <c r="AQ8"/>
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="30"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="37"/>
+      <c r="H9" s="21"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1407,18 +1233,18 @@
       <c r="AQ9"/>
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="55"/>
+      <c r="A10" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="33"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1456,18 +1282,18 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="18">
-        <v>44866</v>
-      </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="55"/>
+      <c r="A11" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="26"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1505,18 +1331,18 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="18">
-        <v>44927</v>
-      </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="56"/>
+      <c r="A12" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="33"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1554,18 +1380,18 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="18">
-        <v>44986</v>
-      </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="55"/>
+      <c r="A13" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="27"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1603,18 +1429,18 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="56"/>
+      <c r="A14" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="33"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1652,18 +1478,18 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="18">
-        <v>45017</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="56"/>
+      <c r="A15" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="33"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1701,18 +1527,18 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="9">
-        <v>44866</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="56"/>
+      <c r="A16" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="21"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1750,16 +1576,18 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="3"/>
+      <c r="A17" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="49" t="s">
+        <v>66</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="57"/>
+      <c r="F17" s="28"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="40"/>
+      <c r="H17" s="33"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1797,16 +1625,18 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="3"/>
+      <c r="A18" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>55</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="40"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1844,16 +1674,18 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="37"/>
+      <c r="A19" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="33"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1891,16 +1723,18 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="37"/>
+      <c r="A20" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="33"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1938,16 +1772,18 @@
       <c r="AQ20"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="52"/>
+      <c r="A21" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="33"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -1985,16 +1821,18 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="A22" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="29"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="33"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -2032,16 +1870,18 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="3"/>
+      <c r="A23" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>59</v>
+      </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="F23" s="31"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="H23" s="33"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2079,16 +1919,18 @@
       <c r="AQ23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="A24" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="29"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="33"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2126,14 +1968,18 @@
       <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
-      <c r="B25" s="3"/>
+      <c r="A25" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="49" t="s">
+        <v>60</v>
+      </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="23"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2171,16 +2017,18 @@
       <c r="AQ25"/>
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="A26" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="29"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="33"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2218,16 +2066,18 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="3"/>
+      <c r="A27" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>62</v>
+      </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="33"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2265,16 +2115,18 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="3"/>
+      <c r="A28" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>63</v>
+      </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="33"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2311,17 +2163,17 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A29" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="36"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2359,16 +2211,16 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="53" t="s">
-        <v>62</v>
-      </c>
+      <c r="A30" s="22"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
+      <c r="C30" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="57"/>
+      <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+      <c r="H30" s="23"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2406,16 +2258,18 @@
       <c r="AQ30"/>
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="A31" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="32"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="33"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2453,16 +2307,18 @@
       <c r="AQ31"/>
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="3"/>
+      <c r="A32" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="49" t="s">
+        <v>70</v>
+      </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="33"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2500,16 +2356,18 @@
       <c r="AQ32"/>
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="A33" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="23"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2546,17 +2404,15 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A34" s="58" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="59"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="60"/>
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="21"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2593,17 +2449,17 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="39"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="40"/>
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A35" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="36"/>
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>
@@ -2640,834 +2496,68 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="41" t="s">
-        <v>41</v>
-      </c>
+    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="20"/>
+      <c r="C36" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="38"/>
-      <c r="I36"/>
-      <c r="J36"/>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="M36"/>
-      <c r="N36"/>
-      <c r="O36"/>
-      <c r="P36"/>
-      <c r="Q36"/>
-      <c r="R36"/>
-      <c r="S36"/>
-      <c r="T36"/>
-      <c r="U36"/>
-      <c r="V36"/>
-      <c r="W36"/>
-      <c r="X36"/>
-      <c r="Y36"/>
-      <c r="Z36"/>
-      <c r="AA36"/>
-      <c r="AB36"/>
-      <c r="AC36"/>
-      <c r="AD36"/>
-      <c r="AE36"/>
-      <c r="AF36"/>
-      <c r="AG36"/>
-      <c r="AH36"/>
-      <c r="AI36"/>
-      <c r="AJ36"/>
-      <c r="AK36"/>
-      <c r="AL36"/>
-      <c r="AM36"/>
-      <c r="AN36"/>
-      <c r="AO36"/>
-      <c r="AP36"/>
-      <c r="AQ36"/>
-    </row>
-    <row r="37" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="40"/>
-      <c r="I37"/>
-      <c r="J37"/>
-      <c r="K37"/>
-      <c r="L37"/>
-      <c r="M37"/>
-      <c r="N37"/>
-      <c r="O37"/>
-      <c r="P37"/>
-      <c r="Q37"/>
-      <c r="R37"/>
-      <c r="S37"/>
-      <c r="T37"/>
-      <c r="U37"/>
-      <c r="V37"/>
-      <c r="W37"/>
-      <c r="X37"/>
-      <c r="Y37"/>
-      <c r="Z37"/>
-      <c r="AA37"/>
-      <c r="AB37"/>
-      <c r="AC37"/>
-      <c r="AD37"/>
-      <c r="AE37"/>
-      <c r="AF37"/>
-      <c r="AG37"/>
-      <c r="AH37"/>
-      <c r="AI37"/>
-      <c r="AJ37"/>
-      <c r="AK37"/>
-      <c r="AL37"/>
-      <c r="AM37"/>
-      <c r="AN37"/>
-      <c r="AO37"/>
-      <c r="AP37"/>
-      <c r="AQ37"/>
-    </row>
-    <row r="38" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="41" t="s">
-        <v>42</v>
-      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="23"/>
+    </row>
+    <row r="37" spans="1:43" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="33"/>
+    </row>
+    <row r="38" spans="1:43" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="40"/>
-      <c r="I38"/>
-      <c r="J38"/>
-      <c r="K38"/>
-      <c r="L38"/>
-      <c r="M38"/>
-      <c r="N38"/>
-      <c r="O38"/>
-      <c r="P38"/>
-      <c r="Q38"/>
-      <c r="R38"/>
-      <c r="S38"/>
-      <c r="T38"/>
-      <c r="U38"/>
-      <c r="V38"/>
-      <c r="W38"/>
-      <c r="X38"/>
-      <c r="Y38"/>
-      <c r="Z38"/>
-      <c r="AA38"/>
-      <c r="AB38"/>
-      <c r="AC38"/>
-      <c r="AD38"/>
-      <c r="AE38"/>
-      <c r="AF38"/>
-      <c r="AG38"/>
-      <c r="AH38"/>
-      <c r="AI38"/>
-      <c r="AJ38"/>
-      <c r="AK38"/>
-      <c r="AL38"/>
-      <c r="AM38"/>
-      <c r="AN38"/>
-      <c r="AO38"/>
-      <c r="AP38"/>
-      <c r="AQ38"/>
-    </row>
-    <row r="39" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="36"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="37"/>
-      <c r="I39"/>
-      <c r="J39"/>
-      <c r="K39"/>
-      <c r="L39"/>
-      <c r="M39"/>
-      <c r="N39"/>
-      <c r="O39"/>
-      <c r="P39"/>
-      <c r="Q39"/>
-      <c r="R39"/>
-      <c r="S39"/>
-      <c r="T39"/>
-      <c r="U39"/>
-      <c r="V39"/>
-      <c r="W39"/>
-      <c r="X39"/>
-      <c r="Y39"/>
-      <c r="Z39"/>
-      <c r="AA39"/>
-      <c r="AB39"/>
-      <c r="AC39"/>
-      <c r="AD39"/>
-      <c r="AE39"/>
-      <c r="AF39"/>
-      <c r="AG39"/>
-      <c r="AH39"/>
-      <c r="AI39"/>
-      <c r="AJ39"/>
-      <c r="AK39"/>
-      <c r="AL39"/>
-      <c r="AM39"/>
-      <c r="AN39"/>
-      <c r="AO39"/>
-      <c r="AP39"/>
-      <c r="AQ39"/>
-    </row>
-    <row r="40" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="36"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="37"/>
-      <c r="I40"/>
-      <c r="J40"/>
-      <c r="K40"/>
-      <c r="L40"/>
-      <c r="M40"/>
-      <c r="N40"/>
-      <c r="O40"/>
-      <c r="P40"/>
-      <c r="Q40"/>
-      <c r="R40"/>
-      <c r="S40"/>
-      <c r="T40"/>
-      <c r="U40"/>
-      <c r="V40"/>
-      <c r="W40"/>
-      <c r="X40"/>
-      <c r="Y40"/>
-      <c r="Z40"/>
-      <c r="AA40"/>
-      <c r="AB40"/>
-      <c r="AC40"/>
-      <c r="AD40"/>
-      <c r="AE40"/>
-      <c r="AF40"/>
-      <c r="AG40"/>
-      <c r="AH40"/>
-      <c r="AI40"/>
-      <c r="AJ40"/>
-      <c r="AK40"/>
-      <c r="AL40"/>
-      <c r="AM40"/>
-      <c r="AN40"/>
-      <c r="AO40"/>
-      <c r="AP40"/>
-      <c r="AQ40"/>
-    </row>
-    <row r="41" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="36"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="37"/>
-      <c r="I41"/>
-      <c r="J41"/>
-      <c r="K41"/>
-      <c r="L41"/>
-      <c r="M41"/>
-      <c r="N41"/>
-      <c r="O41"/>
-      <c r="P41"/>
-      <c r="Q41"/>
-      <c r="R41"/>
-      <c r="S41"/>
-      <c r="T41"/>
-      <c r="U41"/>
-      <c r="V41"/>
-      <c r="W41"/>
-      <c r="X41"/>
-      <c r="Y41"/>
-      <c r="Z41"/>
-      <c r="AA41"/>
-      <c r="AB41"/>
-      <c r="AC41"/>
-      <c r="AD41"/>
-      <c r="AE41"/>
-      <c r="AF41"/>
-      <c r="AG41"/>
-      <c r="AH41"/>
-      <c r="AI41"/>
-      <c r="AJ41"/>
-      <c r="AK41"/>
-      <c r="AL41"/>
-      <c r="AM41"/>
-      <c r="AN41"/>
-      <c r="AO41"/>
-      <c r="AP41"/>
-      <c r="AQ41"/>
-    </row>
-    <row r="42" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="35"/>
-      <c r="I42"/>
-      <c r="J42"/>
-      <c r="K42"/>
-      <c r="L42"/>
-      <c r="M42"/>
-      <c r="N42"/>
-      <c r="O42"/>
-      <c r="P42"/>
-      <c r="Q42"/>
-      <c r="R42"/>
-      <c r="S42"/>
-      <c r="T42"/>
-      <c r="U42"/>
-      <c r="V42"/>
-      <c r="W42"/>
-      <c r="X42"/>
-      <c r="Y42"/>
-      <c r="Z42"/>
-      <c r="AA42"/>
-      <c r="AB42"/>
-      <c r="AC42"/>
-      <c r="AD42"/>
-      <c r="AE42"/>
-      <c r="AF42"/>
-      <c r="AG42"/>
-      <c r="AH42"/>
-      <c r="AI42"/>
-      <c r="AJ42"/>
-      <c r="AK42"/>
-      <c r="AL42"/>
-      <c r="AM42"/>
-      <c r="AN42"/>
-      <c r="AO42"/>
-      <c r="AP42"/>
-      <c r="AQ42"/>
-    </row>
-    <row r="43" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="18">
-        <v>45200</v>
-      </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="37"/>
-      <c r="I43"/>
-      <c r="J43"/>
-      <c r="K43"/>
-      <c r="L43"/>
-      <c r="M43"/>
-      <c r="N43"/>
-      <c r="O43"/>
-      <c r="P43"/>
-      <c r="Q43"/>
-      <c r="R43"/>
-      <c r="S43"/>
-      <c r="T43"/>
-      <c r="U43"/>
-      <c r="V43"/>
-      <c r="W43"/>
-      <c r="X43"/>
-      <c r="Y43"/>
-      <c r="Z43"/>
-      <c r="AA43"/>
-      <c r="AB43"/>
-      <c r="AC43"/>
-      <c r="AD43"/>
-      <c r="AE43"/>
-      <c r="AF43"/>
-      <c r="AG43"/>
-      <c r="AH43"/>
-      <c r="AI43"/>
-      <c r="AJ43"/>
-      <c r="AK43"/>
-      <c r="AL43"/>
-      <c r="AM43"/>
-      <c r="AN43"/>
-      <c r="AO43"/>
-      <c r="AP43"/>
-      <c r="AQ43"/>
-    </row>
-    <row r="44" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="18">
-        <v>45200</v>
-      </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="37"/>
-      <c r="I44"/>
-      <c r="J44"/>
-      <c r="K44"/>
-      <c r="L44"/>
-      <c r="M44"/>
-      <c r="N44"/>
-      <c r="O44"/>
-      <c r="P44"/>
-      <c r="Q44"/>
-      <c r="R44"/>
-      <c r="S44"/>
-      <c r="T44"/>
-      <c r="U44"/>
-      <c r="V44"/>
-      <c r="W44"/>
-      <c r="X44"/>
-      <c r="Y44"/>
-      <c r="Z44"/>
-      <c r="AA44"/>
-      <c r="AB44"/>
-      <c r="AC44"/>
-      <c r="AD44"/>
-      <c r="AE44"/>
-      <c r="AF44"/>
-      <c r="AG44"/>
-      <c r="AH44"/>
-      <c r="AI44"/>
-      <c r="AJ44"/>
-      <c r="AK44"/>
-      <c r="AL44"/>
-      <c r="AM44"/>
-      <c r="AN44"/>
-      <c r="AO44"/>
-      <c r="AP44"/>
-      <c r="AQ44"/>
-    </row>
-    <row r="45" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="38"/>
-      <c r="I45"/>
-      <c r="J45"/>
-      <c r="K45"/>
-      <c r="L45"/>
-      <c r="M45"/>
-      <c r="N45"/>
-      <c r="O45"/>
-      <c r="P45"/>
-      <c r="Q45"/>
-      <c r="R45"/>
-      <c r="S45"/>
-      <c r="T45"/>
-      <c r="U45"/>
-      <c r="V45"/>
-      <c r="W45"/>
-      <c r="X45"/>
-      <c r="Y45"/>
-      <c r="Z45"/>
-      <c r="AA45"/>
-      <c r="AB45"/>
-      <c r="AC45"/>
-      <c r="AD45"/>
-      <c r="AE45"/>
-      <c r="AF45"/>
-      <c r="AG45"/>
-      <c r="AH45"/>
-      <c r="AI45"/>
-      <c r="AJ45"/>
-      <c r="AK45"/>
-      <c r="AL45"/>
-      <c r="AM45"/>
-      <c r="AN45"/>
-      <c r="AO45"/>
-      <c r="AP45"/>
-      <c r="AQ45"/>
-    </row>
-    <row r="46" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="38"/>
-      <c r="I46"/>
-      <c r="J46"/>
-      <c r="K46"/>
-      <c r="L46"/>
-      <c r="M46"/>
-      <c r="N46"/>
-      <c r="O46"/>
-      <c r="P46"/>
-      <c r="Q46"/>
-      <c r="R46"/>
-      <c r="S46"/>
-      <c r="T46"/>
-      <c r="U46"/>
-      <c r="V46"/>
-      <c r="W46"/>
-      <c r="X46"/>
-      <c r="Y46"/>
-      <c r="Z46"/>
-      <c r="AA46"/>
-      <c r="AB46"/>
-      <c r="AC46"/>
-      <c r="AD46"/>
-      <c r="AE46"/>
-      <c r="AF46"/>
-      <c r="AG46"/>
-      <c r="AH46"/>
-      <c r="AI46"/>
-      <c r="AJ46"/>
-      <c r="AK46"/>
-      <c r="AL46"/>
-      <c r="AM46"/>
-      <c r="AN46"/>
-      <c r="AO46"/>
-      <c r="AP46"/>
-      <c r="AQ46"/>
-    </row>
-    <row r="47" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="38"/>
-      <c r="I47"/>
-      <c r="J47"/>
-      <c r="K47"/>
-      <c r="L47"/>
-      <c r="M47"/>
-      <c r="N47"/>
-      <c r="O47"/>
-      <c r="P47"/>
-      <c r="Q47"/>
-      <c r="R47"/>
-      <c r="S47"/>
-      <c r="T47"/>
-      <c r="U47"/>
-      <c r="V47"/>
-      <c r="W47"/>
-      <c r="X47"/>
-      <c r="Y47"/>
-      <c r="Z47"/>
-      <c r="AA47"/>
-      <c r="AB47"/>
-      <c r="AC47"/>
-      <c r="AD47"/>
-      <c r="AE47"/>
-      <c r="AF47"/>
-      <c r="AG47"/>
-      <c r="AH47"/>
-      <c r="AI47"/>
-      <c r="AJ47"/>
-      <c r="AK47"/>
-      <c r="AL47"/>
-      <c r="AM47"/>
-      <c r="AN47"/>
-      <c r="AO47"/>
-      <c r="AP47"/>
-      <c r="AQ47"/>
-    </row>
-    <row r="48" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="38"/>
-      <c r="I48"/>
-      <c r="J48"/>
-      <c r="K48"/>
-      <c r="L48"/>
-      <c r="M48"/>
-      <c r="N48"/>
-      <c r="O48"/>
-      <c r="P48"/>
-      <c r="Q48"/>
-      <c r="R48"/>
-      <c r="S48"/>
-      <c r="T48"/>
-      <c r="U48"/>
-      <c r="V48"/>
-      <c r="W48"/>
-      <c r="X48"/>
-      <c r="Y48"/>
-      <c r="Z48"/>
-      <c r="AA48"/>
-      <c r="AB48"/>
-      <c r="AC48"/>
-      <c r="AD48"/>
-      <c r="AE48"/>
-      <c r="AF48"/>
-      <c r="AG48"/>
-      <c r="AH48"/>
-      <c r="AI48"/>
-      <c r="AJ48"/>
-      <c r="AK48"/>
-      <c r="AL48"/>
-      <c r="AM48"/>
-      <c r="AN48"/>
-      <c r="AO48"/>
-      <c r="AP48"/>
-      <c r="AQ48"/>
-    </row>
-    <row r="49" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="38"/>
-      <c r="I49"/>
-      <c r="J49"/>
-      <c r="K49"/>
-      <c r="L49"/>
-      <c r="M49"/>
-      <c r="N49"/>
-      <c r="O49"/>
-      <c r="P49"/>
-      <c r="Q49"/>
-      <c r="R49"/>
-      <c r="S49"/>
-      <c r="T49"/>
-      <c r="U49"/>
-      <c r="V49"/>
-      <c r="W49"/>
-      <c r="X49"/>
-      <c r="Y49"/>
-      <c r="Z49"/>
-      <c r="AA49"/>
-      <c r="AB49"/>
-      <c r="AC49"/>
-      <c r="AD49"/>
-      <c r="AE49"/>
-      <c r="AF49"/>
-      <c r="AG49"/>
-      <c r="AH49"/>
-      <c r="AI49"/>
-      <c r="AJ49"/>
-      <c r="AK49"/>
-      <c r="AL49"/>
-      <c r="AM49"/>
-      <c r="AN49"/>
-      <c r="AO49"/>
-      <c r="AP49"/>
-      <c r="AQ49"/>
-    </row>
-    <row r="50" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="39"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="37"/>
-      <c r="I50"/>
-      <c r="J50"/>
-      <c r="K50"/>
-      <c r="L50"/>
-      <c r="M50"/>
-      <c r="N50"/>
-      <c r="O50"/>
-      <c r="P50"/>
-      <c r="Q50"/>
-      <c r="R50"/>
-      <c r="S50"/>
-      <c r="T50"/>
-      <c r="U50"/>
-      <c r="V50"/>
-      <c r="W50"/>
-      <c r="X50"/>
-      <c r="Y50"/>
-      <c r="Z50"/>
-      <c r="AA50"/>
-      <c r="AB50"/>
-      <c r="AC50"/>
-      <c r="AD50"/>
-      <c r="AE50"/>
-      <c r="AF50"/>
-      <c r="AG50"/>
-      <c r="AH50"/>
-      <c r="AI50"/>
-      <c r="AJ50"/>
-      <c r="AK50"/>
-      <c r="AL50"/>
-      <c r="AM50"/>
-      <c r="AN50"/>
-      <c r="AO50"/>
-      <c r="AP50"/>
-      <c r="AQ50"/>
-    </row>
-    <row r="51" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A51" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" s="48"/>
-      <c r="C51" s="48"/>
-      <c r="D51" s="48"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="49"/>
-      <c r="I51"/>
-      <c r="J51"/>
-      <c r="K51"/>
-      <c r="L51"/>
-      <c r="M51"/>
-      <c r="N51"/>
-      <c r="O51"/>
-      <c r="P51"/>
-      <c r="Q51"/>
-      <c r="R51"/>
-      <c r="S51"/>
-      <c r="T51"/>
-      <c r="U51"/>
-      <c r="V51"/>
-      <c r="W51"/>
-      <c r="X51"/>
-      <c r="Y51"/>
-      <c r="Z51"/>
-      <c r="AA51"/>
-      <c r="AB51"/>
-      <c r="AC51"/>
-      <c r="AD51"/>
-      <c r="AE51"/>
-      <c r="AF51"/>
-      <c r="AG51"/>
-      <c r="AH51"/>
-      <c r="AI51"/>
-      <c r="AJ51"/>
-      <c r="AK51"/>
-      <c r="AL51"/>
-      <c r="AM51"/>
-      <c r="AN51"/>
-      <c r="AO51"/>
-      <c r="AP51"/>
-      <c r="AQ51"/>
-    </row>
-    <row r="52" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="39"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="40"/>
-    </row>
-    <row r="53" spans="1:43" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A53" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="40"/>
-    </row>
-    <row r="54" spans="1:43" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A54" s="41"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="42"/>
-    </row>
-    <row r="55" spans="1:43" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A55" s="41"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="40"/>
-    </row>
-    <row r="56" spans="1:43" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A56" s="36"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="37"/>
-    </row>
-    <row r="57" spans="1:43" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A57" s="36"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="37"/>
-    </row>
-    <row r="58" spans="1:43" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="43"/>
-      <c r="B58" s="44"/>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="46"/>
-    </row>
-    <row r="59" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="25"/>
+    </row>
+    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -3481,29 +2571,9 @@
     <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A51:H51"/>
+  <mergeCells count="12">
+    <mergeCell ref="A35:H35"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:E3"/>
@@ -3512,15 +2582,14 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A42:H42"/>
+    <mergeCell ref="A29:H29"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="52" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="49" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>